<commit_message>
Abatement can solve in B-mode with sumU and sumX
</commit_message>
<xml_diff>
--- a/examples/Abatement/Data/techdata_new.xlsx
+++ b/examples/Abatement/Data/techdata_new.xlsx
@@ -639,8 +639,8 @@
   <dimension ref="A1:AJ6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R5" sqref="R5"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
EOP runs as part of the abate class.
This commit is the last one before we split into 2 classes
</commit_message>
<xml_diff>
--- a/examples/Abatement/Data/techdata_new.xlsx
+++ b/examples/Abatement/Data/techdata_new.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12300" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="inputdisp" sheetId="1" r:id="rId1"/>
@@ -638,7 +638,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="C15" sqref="C15"/>
     </sheetView>
@@ -1352,9 +1352,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H27" sqref="H27"/>
+      <selection pane="topRight" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>